<commit_message>
features-implemented of upload question list from excel file
</commit_message>
<xml_diff>
--- a/controller/Quiz_controller/myfile.xlsx
+++ b/controller/Quiz_controller/myfile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gyan Backend\Gyan Backend\gyan-backend\controller\Quiz_controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA989761-1520-4BB8-9089-9AC9087808EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B557D6-7450-4FD0-9572-BC8DEB013CF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2E798114-F9CE-47F6-AC26-6FB15606552D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="64">
   <si>
     <t>title</t>
   </si>
@@ -51,56 +51,179 @@
     <t>chapter</t>
   </si>
   <si>
-    <t>correct options</t>
+    <t>दंत विशेषज्ञ किस दर्पण का उपयोग मरीजों के दाँतों का बड़ा प्रतिबिंब देखने के लिए करता है?</t>
   </si>
   <si>
-    <t>xyz</t>
+    <t>समतल दर्पण</t>
   </si>
   <si>
-    <t>ab</t>
+    <t>अवतल दर्पण</t>
   </si>
   <si>
-    <t>bc</t>
+    <t>उत्तल दर्पण</t>
   </si>
   <si>
-    <t>cd</t>
+    <t>इनमें से सभी</t>
   </si>
   <si>
-    <t>de</t>
+    <t>Science</t>
   </si>
   <si>
-    <t>Physics</t>
+    <t>कौन-सा लेंस अपसारी लेंस भी कहलाता है?</t>
   </si>
   <si>
-    <t>electric</t>
+    <t>अवतल लेंस</t>
   </si>
   <si>
-    <t>opion1,option2</t>
+    <t>उत्तल लेंस</t>
   </si>
   <si>
-    <t>what is lens</t>
+    <t>अवतल एवं उत्तल लेंस दोनों</t>
   </si>
   <si>
-    <t>fiber</t>
+    <t>इनमें से कोई नहीं</t>
   </si>
   <si>
-    <t>table</t>
+    <t xml:space="preserve"> उत्तल लेंस</t>
   </si>
   <si>
-    <t>ee</t>
+    <t>All</t>
   </si>
   <si>
-    <t>dd</t>
+    <t>पुतली के साइज को कौन नियंत्रित करता है?</t>
   </si>
   <si>
-    <t>chemistry</t>
+    <t>पक्ष्माभी</t>
+  </si>
+  <si>
+    <t>परितारिका</t>
+  </si>
+  <si>
+    <t>नेत्र लेंस</t>
+  </si>
+  <si>
+    <t>रेटिना (दृष्टि पटल)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> रेटिना (दृष्टि पटल)</t>
+  </si>
+  <si>
+    <t>किसी दृष्टि दोष को अवतल और उत्तल दोनों लेंसों से बने द्विफोकसी लेंस द्वारा संशोधित किया जा सकता है?</t>
+  </si>
+  <si>
+    <t>निकट दृष्टि दोष</t>
+  </si>
+  <si>
+    <t>दीर्घ-दृष्टि दोष</t>
+  </si>
+  <si>
+    <t>जरा-दूर दृष्टिता</t>
+  </si>
+  <si>
+    <t> मोतियाबिंद</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> मोतियाबिंद</t>
+  </si>
+  <si>
+    <t>एक प्रयोग में अवतल दर्पण द्वारा किसी बिंब का प्रतिबिंब एक पर्दे पर प्राप्त किया जाता है । दर्पण की फोकस दूरी को निर्धारित करने के लिए प्रयोगकर्ता को मापने की जरूरत है</t>
+  </si>
+  <si>
+    <t>दर्पण तथा पर्दा के बीच की दूरी को</t>
+  </si>
+  <si>
+    <t>‘A’ और ‘B’ दोनों</t>
+  </si>
+  <si>
+    <t> इनमें से कोई नहीं</t>
+  </si>
+  <si>
+    <t>दर्पण तथा बिंब के बीच की दूरी को</t>
+  </si>
+  <si>
+    <t>शब्दकोष के छोटे अक्षरों को पढ़ने के लिए किस लेंस का उपयोग करना पसंद करेंगे?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 50 cm फोकस दूरी का अवतल लेंस</t>
+  </si>
+  <si>
+    <t>50 cm फोकस दूरी का उत्तल लेंस</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5 cm फोकस दूरी का उत्तल लेंस</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5 cm फोकस दूरी का अवतल लेंस</t>
+  </si>
+  <si>
+    <t>निम्नलिखित में से कौन विद्युत विभवान्तर का SI मात्रक है?</t>
+  </si>
+  <si>
+    <t>वोल्ट</t>
+  </si>
+  <si>
+    <t>ओम</t>
+  </si>
+  <si>
+    <t>वोल्ट प्रति कूलॉम</t>
+  </si>
+  <si>
+    <t>ऐम्पियर</t>
+  </si>
+  <si>
+    <t>लघुपथन (शार्ट सर्किट) के समय परिपथ में विद्युत धारा का मान</t>
+  </si>
+  <si>
+    <t>बहुत कम हो जाता है</t>
+  </si>
+  <si>
+    <t>परिवर्तित नहीं होता है</t>
+  </si>
+  <si>
+    <t>बहुत अधिक बढ़ जाता है</t>
+  </si>
+  <si>
+    <t>निरंतर परिवर्तित होता है</t>
+  </si>
+  <si>
+    <t>पश्चिम की ओर प्रक्षेपित कोई धनावेशित कण (अल्फा कण) किसी चुंबकीय क्षेत्र द्वारा उत्तर की ओर विक्षेपित हो जाता है। चुंबकीय क्षेत्र की दिशा क्या है?</t>
+  </si>
+  <si>
+    <t>दक्षिण की ओर</t>
+  </si>
+  <si>
+    <t>पूर्व की ओर</t>
+  </si>
+  <si>
+    <t>अधोमुखी</t>
+  </si>
+  <si>
+    <t>उपरिमुखी</t>
+  </si>
+  <si>
+    <t>ताँबे के तार की एक आयताकार कुंडली किसी चुंबकीय क्षेत्र में घूर्णी गति कर रही है। इस कुंडली में प्रेरित विद्युत धारा की दिशा में कितने परिभ्रमण के पश्चात् परिवर्तन होता है</t>
+  </si>
+  <si>
+    <t> दो</t>
+  </si>
+  <si>
+    <t>एक</t>
+  </si>
+  <si>
+    <t>आधे</t>
+  </si>
+  <si>
+    <t>चौथाई</t>
+  </si>
+  <si>
+    <t>correctOptions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,6 +237,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -123,7 +252,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -146,17 +275,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -475,12 +619,23 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="39.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.21875" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" customWidth="1"/>
+    <col min="9" max="9" width="16.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -506,7 +661,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>63</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -528,31 +683,31 @@
     </row>
     <row r="2" spans="1:26" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="F2" s="2">
         <v>10</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -573,31 +728,33 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="F3" s="1">
+        <v>10</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="1">
-        <v>12</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -616,16 +773,34 @@
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
-    <row r="4" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
+    <row r="4" spans="1:26" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="1">
+        <v>10</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -644,16 +819,34 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
     </row>
-    <row r="5" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
+    <row r="5" spans="1:26" ht="42" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="1">
+        <v>10</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -672,16 +865,34 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
     </row>
-    <row r="6" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
+    <row r="6" spans="1:26" ht="55.2" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="1">
+        <v>10</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -700,16 +911,34 @@
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
     </row>
-    <row r="7" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
+    <row r="7" spans="1:26" ht="42" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="1">
+        <v>10</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -728,16 +957,34 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
-    <row r="8" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+    <row r="8" spans="1:26" ht="28.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="1">
+        <v>10</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -756,16 +1003,34 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
     </row>
-    <row r="9" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+    <row r="9" spans="1:26" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="1">
+        <v>10</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -784,16 +1049,34 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
     </row>
-    <row r="10" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+    <row r="10" spans="1:26" ht="55.2" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" s="1">
+        <v>10</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -812,16 +1095,34 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
     </row>
-    <row r="11" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
+    <row r="11" spans="1:26" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="1">
+        <v>10</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>

</xml_diff>